<commit_message>
all sorts of stuff I should've been committing for weeks
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76465C57-1176-4A50-860B-08A602A956B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34F96B0-A59D-44BB-81AC-8C55AE2068CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="2940" windowWidth="20160" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3660" yWindow="2770" windowWidth="30170" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="160">
   <si>
     <t>Key</t>
   </si>
@@ -38,6 +38,468 @@
   </si>
   <si>
     <t>&lt;size=50&gt;Attack on Blob&lt;/size&gt;\nDivide and Conquer</t>
+  </si>
+  <si>
+    <t>enter</t>
+  </si>
+  <si>
+    <t>ENTER</t>
+  </si>
+  <si>
+    <t>Watch out! Once the health bar is empty, you will have to start over!</t>
+  </si>
+  <si>
+    <t>health_warning</t>
+  </si>
+  <si>
+    <t>split</t>
+  </si>
+  <si>
+    <t>SPLIT</t>
+  </si>
+  <si>
+    <t>cancel</t>
+  </si>
+  <si>
+    <t>CANCEL</t>
+  </si>
+  <si>
+    <t>victory</t>
+  </si>
+  <si>
+    <t>VICTORY</t>
+  </si>
+  <si>
+    <t>attacks</t>
+  </si>
+  <si>
+    <t>ATTACKS</t>
+  </si>
+  <si>
+    <t>errors</t>
+  </si>
+  <si>
+    <t>ERRORS</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>SCORE</t>
+  </si>
+  <si>
+    <t>efficient</t>
+  </si>
+  <si>
+    <t>EFFICIENT</t>
+  </si>
+  <si>
+    <t>placeValue</t>
+  </si>
+  <si>
+    <t>Place Value</t>
+  </si>
+  <si>
+    <t>placeValueDistribute</t>
+  </si>
+  <si>
+    <t>Place Value Distribute</t>
+  </si>
+  <si>
+    <t>placeOnes</t>
+  </si>
+  <si>
+    <t>Ones</t>
+  </si>
+  <si>
+    <t>placeTens</t>
+  </si>
+  <si>
+    <t>Tens</t>
+  </si>
+  <si>
+    <t>placeHundreds</t>
+  </si>
+  <si>
+    <t>Hundreds</t>
+  </si>
+  <si>
+    <t>lesson1_intro_1</t>
+  </si>
+  <si>
+    <t>lesson1_intro_0</t>
+  </si>
+  <si>
+    <t>Dividing a large number can be daunting, but with the right trick, it can be a breeze!</t>
+  </si>
+  <si>
+    <t>Let’s briefly examine a useful mathematical principle that will help us.</t>
+  </si>
+  <si>
+    <t>lesson1_placeValue_0</t>
+  </si>
+  <si>
+    <t>First, let’s take a quick look at how large numbers are arranged by single digit numbers.</t>
+  </si>
+  <si>
+    <t>lesson1_placeValue_1</t>
+  </si>
+  <si>
+    <t>These digits are placed by multiples of 10’s, since we use a base 10 number system.</t>
+  </si>
+  <si>
+    <t>lesson1_placeValueDistribute_0</t>
+  </si>
+  <si>
+    <t>lesson1_placeValueDistribute_1</t>
+  </si>
+  <si>
+    <t>lesson1_end_0</t>
+  </si>
+  <si>
+    <t>lesson1_placeValueDistribute_2</t>
+  </si>
+  <si>
+    <t>Now with that in mind, we can split a large number up by this principle.</t>
+  </si>
+  <si>
+    <t>Splitting up a number to be added later is known as the distributive property.</t>
+  </si>
+  <si>
+    <t>Pay close attention to how the distributive property works in this example!</t>
+  </si>
+  <si>
+    <t>Let’s go ahead and put this into practice when we face the first mega blob!</t>
+  </si>
+  <si>
+    <t>areaModel</t>
+  </si>
+  <si>
+    <t>Area Model</t>
+  </si>
+  <si>
+    <t>areaModelDistribute</t>
+  </si>
+  <si>
+    <t>Area Model Distribute</t>
+  </si>
+  <si>
+    <t>lesson2_intro_0</t>
+  </si>
+  <si>
+    <t>lesson2_intro_1</t>
+  </si>
+  <si>
+    <t>lesson2_areaModel_0</t>
+  </si>
+  <si>
+    <t>lesson2_areaModel_1</t>
+  </si>
+  <si>
+    <t>lesson2_areaModelDistribute_0</t>
+  </si>
+  <si>
+    <t>lesson2_areaModelDistribute_1</t>
+  </si>
+  <si>
+    <t>lesson2_areaModelDistribute_2</t>
+  </si>
+  <si>
+    <t>lesson2_end_0</t>
+  </si>
+  <si>
+    <t>This time around, we will be dividing with double-digit numbers.</t>
+  </si>
+  <si>
+    <t>It would be too troublesome to deal with these blobs using our current technique.</t>
+  </si>
+  <si>
+    <t>Fortunately, we have one more trick our sleeves!</t>
+  </si>
+  <si>
+    <t>lesson2_intro_2</t>
+  </si>
+  <si>
+    <t>Since division is the inverse of multiplication, you can visualize the equation as the dimensions of an area.</t>
+  </si>
+  <si>
+    <t>In this case, the answer to the equation is the width of the area.</t>
+  </si>
+  <si>
+    <t>We can then use this model to partially solve the equation with smaller numbers.</t>
+  </si>
+  <si>
+    <t>Observe how the area is being split into two.</t>
+  </si>
+  <si>
+    <t>Adding the two split values will then give you the whole solution.</t>
+  </si>
+  <si>
+    <t>Now why don’t we try this new technique out with the next mega blob!</t>
+  </si>
+  <si>
+    <t>level1_intro_0</t>
+  </si>
+  <si>
+    <t>Look out! Two blobs have appeared.</t>
+  </si>
+  <si>
+    <t>level1_intro_1</t>
+  </si>
+  <si>
+    <t>level1_intro_2</t>
+  </si>
+  <si>
+    <t>level1_intro_3</t>
+  </si>
+  <si>
+    <t>In order to attack the mega blob, we must merge all the blobs into one golden blob.</t>
+  </si>
+  <si>
+    <t>That means finding the quotient of the division between the two present numbers.</t>
+  </si>
+  <si>
+    <t>Those numbers don’t look that scary. We can directly divide those numbers.</t>
+  </si>
+  <si>
+    <t>instruct_drag_blob_0</t>
+  </si>
+  <si>
+    <t>In order to merge the two blobs, simply drag one to another like so.</t>
+  </si>
+  <si>
+    <t>op_instruct_0</t>
+  </si>
+  <si>
+    <t>op_instruct_1</t>
+  </si>
+  <si>
+    <t>op_instruct_2</t>
+  </si>
+  <si>
+    <t>Now you must solve the operation by typing in the number via the numpad.</t>
+  </si>
+  <si>
+    <t>You can also use the keyboard to enter the numbers.</t>
+  </si>
+  <si>
+    <t>Once you feel confident with your answer, press the ENTER button on the numpad (or your keyboard).</t>
+  </si>
+  <si>
+    <t>Excellent! Our attack on the mega blob was a success!</t>
+  </si>
+  <si>
+    <t>attack_instruct_success_0</t>
+  </si>
+  <si>
+    <t>attack_instruct_boss_hp_0</t>
+  </si>
+  <si>
+    <t>attack_instruct_boss_hp_1</t>
+  </si>
+  <si>
+    <t>attack_instruct_boss_hp_2</t>
+  </si>
+  <si>
+    <t>This is the representation of the mega blob’s health.</t>
+  </si>
+  <si>
+    <t>As you can see, it has been reduced.</t>
+  </si>
+  <si>
+    <t>Once it’s empty, the mega blob will be defeated.</t>
+  </si>
+  <si>
+    <t>split_instruct_0</t>
+  </si>
+  <si>
+    <t>split_instruct_1</t>
+  </si>
+  <si>
+    <t>split_instruct_2</t>
+  </si>
+  <si>
+    <t>Here you can see a representation of how the blob is going to be split.</t>
+  </si>
+  <si>
+    <t>We will be splitting the blob by transferring its digits to a new blob.</t>
+  </si>
+  <si>
+    <t>Now we are dealing with a much larger blob!</t>
+  </si>
+  <si>
+    <t>Let’s split the blob up into two to make our life easier.</t>
+  </si>
+  <si>
+    <t>Press the sparkly blob as shown to proceed.</t>
+  </si>
+  <si>
+    <t>split_op_instruct_0</t>
+  </si>
+  <si>
+    <t>split_op_instruct_1</t>
+  </si>
+  <si>
+    <t>split_op_instruct_2</t>
+  </si>
+  <si>
+    <t>split_op_instruct_3</t>
+  </si>
+  <si>
+    <t>split_op_instruct_4</t>
+  </si>
+  <si>
+    <t>Simply click on any of the digits to transfer them.</t>
+  </si>
+  <si>
+    <t>Once you are happy with the new split numbers, press the SPLIT button.</t>
+  </si>
+  <si>
+    <t>Remember, both new numbers must be wholly divisible for the split to succeed!</t>
+  </si>
+  <si>
+    <t>split_op_success_0</t>
+  </si>
+  <si>
+    <t>split_op_success_1</t>
+  </si>
+  <si>
+    <t>split_op_success_2</t>
+  </si>
+  <si>
+    <t>Nicely done! The blobs have now been split into two smaller numbers.</t>
+  </si>
+  <si>
+    <t>You can split the numbers further if you want, but there’s a limit!</t>
+  </si>
+  <si>
+    <t>Once you have solved all the blobs, you can merge them into one golden blob for an attack.</t>
+  </si>
+  <si>
+    <t>split_op_success_3</t>
+  </si>
+  <si>
+    <t>Good luck!</t>
+  </si>
+  <si>
+    <t>level3_intro_0</t>
+  </si>
+  <si>
+    <t>Watch out! These blobs are not to be trifled with!</t>
+  </si>
+  <si>
+    <t>split_instruct2_0</t>
+  </si>
+  <si>
+    <t>Just as you have done many times before, go ahead a press the sparkly blob.</t>
+  </si>
+  <si>
+    <t>split_op_partial_instruct_0</t>
+  </si>
+  <si>
+    <t>split_op_partial_instruct_1</t>
+  </si>
+  <si>
+    <t>Here we are going to reduce the blob’s large number by multiply the divisor for a certain amount.</t>
+  </si>
+  <si>
+    <t>First you must specify the number to multiply for the divisor. Simply type in the number, and press ENTER.</t>
+  </si>
+  <si>
+    <t>split_op_partial_next_instruct_0</t>
+  </si>
+  <si>
+    <t>split_op_partial_next_instruct_1</t>
+  </si>
+  <si>
+    <t>split_op_partial_next_instruct_2</t>
+  </si>
+  <si>
+    <t>Now you must type in the correct number that multiplies the two numbers.</t>
+  </si>
+  <si>
+    <t>Once you press ENTER, you’ll see that number subtracted from the dividend blob.</t>
+  </si>
+  <si>
+    <t>If the resulting value is less than zero, then try again with a smaller multiplication number!</t>
+  </si>
+  <si>
+    <t>split_op_partial_success_0</t>
+  </si>
+  <si>
+    <t>split_op_partial_success_1</t>
+  </si>
+  <si>
+    <t>split_op_partial_success_2</t>
+  </si>
+  <si>
+    <t>Good! The blob’s value has been reduced, and a partial quotient blob has appeared.</t>
+  </si>
+  <si>
+    <t>Splitting up large numbers this way makes it easier to deal with two or more-digit divisors!</t>
+  </si>
+  <si>
+    <t>I’ve said all that I can to help you, now go forth and defeat the rest of these mega blobs!</t>
+  </si>
+  <si>
+    <t>options</t>
+  </si>
+  <si>
+    <t>music</t>
+  </si>
+  <si>
+    <t>sound</t>
+  </si>
+  <si>
+    <t>speech</t>
+  </si>
+  <si>
+    <t>close</t>
+  </si>
+  <si>
+    <t>on</t>
+  </si>
+  <si>
+    <t>off</t>
+  </si>
+  <si>
+    <t>OPTIONS</t>
+  </si>
+  <si>
+    <t>MUSIC</t>
+  </si>
+  <si>
+    <t>SOUND</t>
+  </si>
+  <si>
+    <t>SPEECH</t>
+  </si>
+  <si>
+    <t>CLOSE</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>OFF</t>
+  </si>
+  <si>
+    <t>credits</t>
+  </si>
+  <si>
+    <t>Made by: RENEGADEWARE</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>continue</t>
+  </si>
+  <si>
+    <t>NEW GAME</t>
+  </si>
+  <si>
+    <t>CONTINUE</t>
   </si>
 </sst>
 </file>
@@ -373,21 +835,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" customWidth="1"/>
-    <col min="2" max="2" width="85.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="35.453125" customWidth="1"/>
+    <col min="2" max="2" width="85.453125" customWidth="1"/>
+    <col min="3" max="3" width="20.26953125" customWidth="1"/>
+    <col min="4" max="4" width="15.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -401,12 +863,628 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>144</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>146</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>72</v>
+      </c>
+      <c r="B46" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>74</v>
+      </c>
+      <c r="B47" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>75</v>
+      </c>
+      <c r="B48" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>76</v>
+      </c>
+      <c r="B49" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>80</v>
+      </c>
+      <c r="B50" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>82</v>
+      </c>
+      <c r="B51" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>83</v>
+      </c>
+      <c r="B52" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>84</v>
+      </c>
+      <c r="B53" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>89</v>
+      </c>
+      <c r="B54" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>90</v>
+      </c>
+      <c r="B55" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>91</v>
+      </c>
+      <c r="B56" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>92</v>
+      </c>
+      <c r="B57" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>96</v>
+      </c>
+      <c r="B58" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>97</v>
+      </c>
+      <c r="B59" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>98</v>
+      </c>
+      <c r="B60" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>104</v>
+      </c>
+      <c r="B61" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>105</v>
+      </c>
+      <c r="B62" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>106</v>
+      </c>
+      <c r="B63" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>107</v>
+      </c>
+      <c r="B64" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>108</v>
+      </c>
+      <c r="B65" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>112</v>
+      </c>
+      <c r="B66" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>113</v>
+      </c>
+      <c r="B67" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>114</v>
+      </c>
+      <c r="B68" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>118</v>
+      </c>
+      <c r="B69" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>120</v>
+      </c>
+      <c r="B70" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>122</v>
+      </c>
+      <c r="B71" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>124</v>
+      </c>
+      <c r="B72" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>125</v>
+      </c>
+      <c r="B73" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>128</v>
+      </c>
+      <c r="B74" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>129</v>
+      </c>
+      <c r="B75" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>130</v>
+      </c>
+      <c r="B76" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>134</v>
+      </c>
+      <c r="B77" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>135</v>
+      </c>
+      <c r="B78" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>136</v>
+      </c>
+      <c r="B79" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a bunch of stuff for initial submission. note to self: still need a bunch of tweaks!
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBCD680B-2D39-49AF-B180-8A92DB0017ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83AF37F2-F349-4FF5-9F6D-A38F280D48F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3830" yWindow="2480" windowWidth="30170" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6300" yWindow="3000" windowWidth="30170" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="186">
   <si>
     <t>Key</t>
   </si>
@@ -133,9 +133,6 @@
     <t>Dividing a large number can be daunting, but with the right trick, it can be a breeze!</t>
   </si>
   <si>
-    <t>Let’s briefly examine a useful mathematical principle that will help us.</t>
-  </si>
-  <si>
     <t>lesson1_placeValue_0</t>
   </si>
   <si>
@@ -160,18 +157,9 @@
     <t>lesson1_placeValueDistribute_2</t>
   </si>
   <si>
-    <t>Now with that in mind, we can split a large number up by this principle.</t>
-  </si>
-  <si>
     <t>Splitting up a number to be added later is known as the distributive property.</t>
   </si>
   <si>
-    <t>Pay close attention to how the distributive property works in this example!</t>
-  </si>
-  <si>
-    <t>Let’s go ahead and put this into practice when we face the first mega blob!</t>
-  </si>
-  <si>
     <t>areaModel</t>
   </si>
   <si>
@@ -208,9 +196,6 @@
     <t>lesson2_end_0</t>
   </si>
   <si>
-    <t>This time around, we will be dividing with double-digit numbers.</t>
-  </si>
-  <si>
     <t>It would be too troublesome to deal with these blobs using our current technique.</t>
   </si>
   <si>
@@ -223,21 +208,9 @@
     <t>Since division is the inverse of multiplication, you can visualize the equation as the dimensions of an area.</t>
   </si>
   <si>
-    <t>In this case, the answer to the equation is the width of the area.</t>
-  </si>
-  <si>
-    <t>We can then use this model to partially solve the equation with smaller numbers.</t>
-  </si>
-  <si>
     <t>Observe how the area is being split into two.</t>
   </si>
   <si>
-    <t>Adding the two split values will then give you the whole solution.</t>
-  </si>
-  <si>
-    <t>Now why don’t we try this new technique out with the next mega blob!</t>
-  </si>
-  <si>
     <t>level1_intro_0</t>
   </si>
   <si>
@@ -250,18 +223,6 @@
     <t>level1_intro_2</t>
   </si>
   <si>
-    <t>level1_intro_3</t>
-  </si>
-  <si>
-    <t>In order to attack the mega blob, we must merge all the blobs into one golden blob.</t>
-  </si>
-  <si>
-    <t>That means finding the quotient of the division between the two present numbers.</t>
-  </si>
-  <si>
-    <t>Those numbers don’t look that scary. We can directly divide those numbers.</t>
-  </si>
-  <si>
     <t>instruct_drag_blob_0</t>
   </si>
   <si>
@@ -367,15 +328,6 @@
     <t>split_op_success_2</t>
   </si>
   <si>
-    <t>Nicely done! The blobs have now been split into two smaller numbers.</t>
-  </si>
-  <si>
-    <t>You can split the numbers further if you want, but there’s a limit!</t>
-  </si>
-  <si>
-    <t>Once you have solved all the blobs, you can merge them into one golden blob for an attack.</t>
-  </si>
-  <si>
     <t>split_op_success_3</t>
   </si>
   <si>
@@ -400,12 +352,6 @@
     <t>split_op_partial_instruct_1</t>
   </si>
   <si>
-    <t>Here we are going to reduce the blob’s large number by multiply the divisor for a certain amount.</t>
-  </si>
-  <si>
-    <t>First you must specify the number to multiply for the divisor. Simply type in the number, and press ENTER.</t>
-  </si>
-  <si>
     <t>split_op_partial_next_instruct_0</t>
   </si>
   <si>
@@ -415,9 +361,6 @@
     <t>split_op_partial_next_instruct_2</t>
   </si>
   <si>
-    <t>Now you must type in the correct number that multiplies the two numbers.</t>
-  </si>
-  <si>
     <t>Once you press ENTER, you’ll see that number subtracted from the dividend blob.</t>
   </si>
   <si>
@@ -436,12 +379,6 @@
     <t>Good! The blob’s value has been reduced, and a partial quotient blob has appeared.</t>
   </si>
   <si>
-    <t>Splitting up large numbers this way makes it easier to deal with two or more-digit divisors!</t>
-  </si>
-  <si>
-    <t>I’ve said all that I can to help you, now go forth and defeat the rest of these mega blobs!</t>
-  </si>
-  <si>
     <t>options</t>
   </si>
   <si>
@@ -584,6 +521,63 @@
   </si>
   <si>
     <t>end_thanks</t>
+  </si>
+  <si>
+    <t>Let’s briefly examine a useful mathematical principle to help us.</t>
+  </si>
+  <si>
+    <t>Now with that in mind, we can split the dividend up by this principle.</t>
+  </si>
+  <si>
+    <t>Pay close attention to how the distributive property works!</t>
+  </si>
+  <si>
+    <t>Let’s go ahead and put this into practice when we face the mega blob!</t>
+  </si>
+  <si>
+    <t>This time around, we will be dividing with double-digit divisors.</t>
+  </si>
+  <si>
+    <t>In this case, the quotient of the division is the width of the area.</t>
+  </si>
+  <si>
+    <t>We can use this model to partially solve the division with smaller numbers.</t>
+  </si>
+  <si>
+    <t>Adding the split values will then give you the whole answer.</t>
+  </si>
+  <si>
+    <t>Now why don’t we try this new technique with the next mega blob!</t>
+  </si>
+  <si>
+    <t>In order to attack the mega blob, we must merge all the blobs into one final quotient blob.</t>
+  </si>
+  <si>
+    <t>Those numbers don’t look that scary. We can directly solve the division.</t>
+  </si>
+  <si>
+    <t>Nicely done! The blobs have now been split into two.</t>
+  </si>
+  <si>
+    <t>You can split the blobs further if you want, but there’s a limit!</t>
+  </si>
+  <si>
+    <t>Once all the blobs have been merged into the final quotient blob, we will be able to attack.</t>
+  </si>
+  <si>
+    <t>Here we are going to reduce the blob’s large number by multiplying the divisor with a number.</t>
+  </si>
+  <si>
+    <t>First you must specify the number to multiply the divisor. Simply type in the number, and press ENTER.</t>
+  </si>
+  <si>
+    <t>Now you must type in the correct answer for the multiplication.</t>
+  </si>
+  <si>
+    <t>Splitting up large numbers this way will make it easier to deal with two or more-digit divisors!</t>
+  </si>
+  <si>
+    <t>I’ve said everything that I can to help you, the rest is up to you. Go forth, and defeat the mega blobs!</t>
   </si>
 </sst>
 </file>
@@ -919,10 +913,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D93"/>
+  <dimension ref="A1:D92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -957,82 +951,82 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>148</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -1149,106 +1143,106 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="B29" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="B30" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="B31" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="B32" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="B33" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="B34" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="B35" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="B36" t="s">
-        <v>175</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="B37" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
       <c r="B38" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="B39" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
@@ -1264,431 +1258,423 @@
         <v>34</v>
       </c>
       <c r="B41" t="s">
-        <v>37</v>
+        <v>167</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" t="s">
         <v>38</v>
-      </c>
-      <c r="B42" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
+        <v>39</v>
+      </c>
+      <c r="B43" t="s">
         <v>40</v>
-      </c>
-      <c r="B43" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44" t="s">
-        <v>46</v>
+        <v>168</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>48</v>
+        <v>169</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B47" t="s">
-        <v>49</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B48" t="s">
-        <v>62</v>
+        <v>171</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B49" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B50" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>67</v>
+        <v>172</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B53" t="s">
-        <v>68</v>
+        <v>173</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B54" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>70</v>
+        <v>174</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B56" t="s">
-        <v>71</v>
+        <v>175</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B57" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B58" t="s">
-        <v>77</v>
+        <v>176</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B59" t="s">
-        <v>78</v>
+        <v>177</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B60" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B61" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B62" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B63" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B64" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B65" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B66" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B67" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B68" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="B69" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="B70" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B71" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="B72" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="B73" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B74" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="B75" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="B76" t="s">
-        <v>111</v>
+        <v>178</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B77" t="s">
-        <v>115</v>
+        <v>179</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="B78" t="s">
-        <v>116</v>
+        <v>180</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="B79" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="B80" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="B81" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B82" t="s">
-        <v>123</v>
+        <v>181</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="B83" t="s">
-        <v>126</v>
+        <v>182</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="B84" t="s">
-        <v>127</v>
+        <v>183</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="B85" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="B86" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="B87" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="B88" t="s">
-        <v>137</v>
+        <v>184</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="B89" t="s">
-        <v>138</v>
+        <v>185</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
       <c r="B90" t="s">
-        <v>139</v>
+        <v>162</v>
+      </c>
+      <c r="C90">
+        <v>2</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="B91" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="C91">
-        <v>2.5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>184</v>
+        <v>166</v>
       </c>
       <c r="B92" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="C92">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
-        <v>187</v>
-      </c>
-      <c r="B93" t="s">
-        <v>186</v>
-      </c>
-      <c r="C93">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed some bugs, gameplay tweaks, graphic tweaks, mockup version, new submit build
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83AF37F2-F349-4FF5-9F6D-A38F280D48F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193EC224-D995-4F35-B851-C5981952152F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6300" yWindow="3000" windowWidth="30170" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4050" yWindow="2000" windowWidth="30170" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="190">
   <si>
     <t>Key</t>
   </si>
@@ -247,9 +247,6 @@
     <t>Once you feel confident with your answer, press the ENTER button on the numpad (or your keyboard).</t>
   </si>
   <si>
-    <t>Excellent! Our attack on the mega blob was a success!</t>
-  </si>
-  <si>
     <t>attack_instruct_success_0</t>
   </si>
   <si>
@@ -550,9 +547,6 @@
     <t>Now why don’t we try this new technique with the next mega blob!</t>
   </si>
   <si>
-    <t>In order to attack the mega blob, we must merge all the blobs into one final quotient blob.</t>
-  </si>
-  <si>
     <t>Those numbers don’t look that scary. We can directly solve the division.</t>
   </si>
   <si>
@@ -578,6 +572,24 @@
   </si>
   <si>
     <t>I’ve said everything that I can to help you, the rest is up to you. Go forth, and defeat the mega blobs!</t>
+  </si>
+  <si>
+    <t>In order to beat the mega blob, we must merge all the blobs into one final quotient blob.</t>
+  </si>
+  <si>
+    <t>Excellent! We’ve managed to clear the blobs!</t>
+  </si>
+  <si>
+    <t>total_errors</t>
+  </si>
+  <si>
+    <t>total_score</t>
+  </si>
+  <si>
+    <t>TOTAL SCORE</t>
+  </si>
+  <si>
+    <t>TOTAL ERROR</t>
   </si>
 </sst>
 </file>
@@ -913,10 +925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D92"/>
+  <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -951,82 +963,82 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -1095,586 +1107,602 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>186</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>189</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>187</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>188</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>145</v>
+        <v>46</v>
       </c>
       <c r="B29" t="s">
-        <v>146</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>139</v>
+        <v>48</v>
       </c>
       <c r="B30" t="s">
-        <v>142</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B31" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
+        <v>138</v>
+      </c>
+      <c r="B32" t="s">
         <v>141</v>
-      </c>
-      <c r="B32" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B33" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B34" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B35" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B36" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B37" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B38" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
+        <v>154</v>
+      </c>
+      <c r="B39" t="s">
         <v>157</v>
-      </c>
-      <c r="B39" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>155</v>
       </c>
       <c r="B40" t="s">
-        <v>36</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>34</v>
+        <v>156</v>
       </c>
       <c r="B41" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B42" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B43" t="s">
-        <v>40</v>
+        <v>166</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B44" t="s">
-        <v>168</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B46" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B47" t="s">
-        <v>170</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B48" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B49" t="s">
-        <v>58</v>
+        <v>169</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>59</v>
+        <v>170</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B52" t="s">
-        <v>172</v>
+        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>173</v>
+        <v>61</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>62</v>
+        <v>171</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>175</v>
+        <v>62</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>64</v>
+        <v>173</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B59" t="s">
-        <v>177</v>
+        <v>64</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B60" t="s">
-        <v>68</v>
+        <v>184</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B61" t="s">
-        <v>72</v>
+        <v>175</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B62" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B63" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B64" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B65" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B66" t="s">
-        <v>81</v>
+        <v>185</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
+        <v>76</v>
+      </c>
+      <c r="B67" t="s">
         <v>79</v>
-      </c>
-      <c r="B67" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B68" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B69" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B70" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B71" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B72" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B73" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B74" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
+        <v>92</v>
+      </c>
+      <c r="B75" t="s">
         <v>95</v>
-      </c>
-      <c r="B75" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B76" t="s">
-        <v>178</v>
+        <v>96</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B77" t="s">
-        <v>179</v>
+        <v>97</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B78" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B79" t="s">
-        <v>103</v>
+        <v>177</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B80" t="s">
-        <v>105</v>
+        <v>178</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B81" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B82" t="s">
-        <v>181</v>
+        <v>104</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B83" t="s">
-        <v>182</v>
+        <v>106</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B84" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B85" t="s">
-        <v>113</v>
+        <v>180</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B86" t="s">
-        <v>114</v>
+        <v>181</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B87" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B88" t="s">
-        <v>184</v>
+        <v>113</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
+        <v>114</v>
+      </c>
+      <c r="B89" t="s">
         <v>117</v>
-      </c>
-      <c r="B89" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>161</v>
+        <v>115</v>
       </c>
       <c r="B90" t="s">
-        <v>162</v>
-      </c>
-      <c r="C90">
-        <v>2</v>
+        <v>182</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>163</v>
+        <v>116</v>
       </c>
       <c r="B91" t="s">
-        <v>164</v>
-      </c>
-      <c r="C91">
-        <v>7</v>
+        <v>183</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B92" t="s">
+        <v>161</v>
+      </c>
+      <c r="C92">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>162</v>
+      </c>
+      <c r="B93" t="s">
+        <v>163</v>
+      </c>
+      <c r="C93">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
         <v>165</v>
       </c>
-      <c r="C92">
+      <c r="B94" t="s">
+        <v>164</v>
+      </c>
+      <c r="C94">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
divisor blob is locked until at least one split, some other fixes
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193EC224-D995-4F35-B851-C5981952152F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBB1245-DA4D-4725-9D9D-6D0EE28A024A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4050" yWindow="2000" windowWidth="30170" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -199,9 +199,6 @@
     <t>It would be too troublesome to deal with these blobs using our current technique.</t>
   </si>
   <si>
-    <t>Fortunately, we have one more trick our sleeves!</t>
-  </si>
-  <si>
     <t>lesson2_intro_2</t>
   </si>
   <si>
@@ -590,6 +587,9 @@
   </si>
   <si>
     <t>TOTAL ERROR</t>
+  </si>
+  <si>
+    <t>Fortunately, we have one more trick up our sleeves!</t>
   </si>
 </sst>
 </file>
@@ -927,8 +927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C93" sqref="C93"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -963,82 +963,82 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -1107,18 +1107,18 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B21" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
+        <v>186</v>
+      </c>
+      <c r="B22" t="s">
         <v>187</v>
-      </c>
-      <c r="B22" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -1187,90 +1187,90 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
+        <v>143</v>
+      </c>
+      <c r="B31" t="s">
         <v>144</v>
-      </c>
-      <c r="B31" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B35" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B36" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B37" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B38" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B39" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B40" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B41" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
@@ -1286,7 +1286,7 @@
         <v>34</v>
       </c>
       <c r="B43" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
@@ -1310,7 +1310,7 @@
         <v>41</v>
       </c>
       <c r="B46" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
@@ -1326,7 +1326,7 @@
         <v>44</v>
       </c>
       <c r="B48" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
@@ -1334,7 +1334,7 @@
         <v>43</v>
       </c>
       <c r="B49" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
@@ -1342,7 +1342,7 @@
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
@@ -1355,10 +1355,10 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B52" t="s">
-        <v>59</v>
+        <v>189</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
@@ -1366,7 +1366,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
@@ -1374,7 +1374,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
@@ -1382,7 +1382,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
@@ -1390,7 +1390,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
@@ -1398,7 +1398,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
@@ -1406,279 +1406,279 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
+        <v>62</v>
+      </c>
+      <c r="B59" t="s">
         <v>63</v>
-      </c>
-      <c r="B59" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B60" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B61" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
+        <v>66</v>
+      </c>
+      <c r="B62" t="s">
         <v>67</v>
-      </c>
-      <c r="B62" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B63" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B64" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B65" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B66" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B67" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B68" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B69" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B70" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B71" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B72" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B73" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B74" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B75" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B76" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B77" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B78" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B79" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B80" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
+        <v>100</v>
+      </c>
+      <c r="B81" t="s">
         <v>101</v>
-      </c>
-      <c r="B81" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
+        <v>102</v>
+      </c>
+      <c r="B82" t="s">
         <v>103</v>
-      </c>
-      <c r="B82" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
+        <v>104</v>
+      </c>
+      <c r="B83" t="s">
         <v>105</v>
-      </c>
-      <c r="B83" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B84" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B85" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B86" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B87" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B88" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B89" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B90" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B91" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
+        <v>159</v>
+      </c>
+      <c r="B92" t="s">
         <v>160</v>
-      </c>
-      <c r="B92" t="s">
-        <v>161</v>
       </c>
       <c r="C92">
         <v>2</v>
@@ -1686,10 +1686,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
+        <v>161</v>
+      </c>
+      <c r="B93" t="s">
         <v>162</v>
-      </c>
-      <c r="B93" t="s">
-        <v>163</v>
       </c>
       <c r="C93">
         <v>5</v>
@@ -1697,10 +1697,10 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B94" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C94">
         <v>2</v>

</xml_diff>

<commit_message>
overhaul partial quotient interface, more interactive lessons
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBB1245-DA4D-4725-9D9D-6D0EE28A024A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7546D10B-5976-431F-AA4E-E136C78A7EEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4050" yWindow="2000" windowWidth="30170" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7420" yWindow="2610" windowWidth="23820" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="214">
   <si>
     <t>Key</t>
   </si>
@@ -142,24 +142,6 @@
     <t>lesson1_placeValue_1</t>
   </si>
   <si>
-    <t>These digits are placed by multiples of 10’s, since we use a base 10 number system.</t>
-  </si>
-  <si>
-    <t>lesson1_placeValueDistribute_0</t>
-  </si>
-  <si>
-    <t>lesson1_placeValueDistribute_1</t>
-  </si>
-  <si>
-    <t>lesson1_end_0</t>
-  </si>
-  <si>
-    <t>lesson1_placeValueDistribute_2</t>
-  </si>
-  <si>
-    <t>Splitting up a number to be added later is known as the distributive property.</t>
-  </si>
-  <si>
     <t>areaModel</t>
   </si>
   <si>
@@ -184,15 +166,6 @@
     <t>lesson2_areaModel_1</t>
   </si>
   <si>
-    <t>lesson2_areaModelDistribute_0</t>
-  </si>
-  <si>
-    <t>lesson2_areaModelDistribute_1</t>
-  </si>
-  <si>
-    <t>lesson2_areaModelDistribute_2</t>
-  </si>
-  <si>
     <t>lesson2_end_0</t>
   </si>
   <si>
@@ -205,9 +178,6 @@
     <t>Since division is the inverse of multiplication, you can visualize the equation as the dimensions of an area.</t>
   </si>
   <si>
-    <t>Observe how the area is being split into two.</t>
-  </si>
-  <si>
     <t>level1_intro_0</t>
   </si>
   <si>
@@ -337,9 +307,6 @@
     <t>split_instruct2_0</t>
   </si>
   <si>
-    <t>Just as you have done many times before, go ahead a press the sparkly blob.</t>
-  </si>
-  <si>
     <t>split_op_partial_instruct_0</t>
   </si>
   <si>
@@ -352,15 +319,9 @@
     <t>split_op_partial_next_instruct_1</t>
   </si>
   <si>
-    <t>split_op_partial_next_instruct_2</t>
-  </si>
-  <si>
     <t>Once you press ENTER, you’ll see that number subtracted from the dividend blob.</t>
   </si>
   <si>
-    <t>If the resulting value is less than zero, then try again with a smaller multiplication number!</t>
-  </si>
-  <si>
     <t>split_op_partial_success_0</t>
   </si>
   <si>
@@ -475,9 +436,6 @@
     <t>Multiple blobs of epic proportion detected!</t>
   </si>
   <si>
-    <t>It seems these blobs came from a lab, and have somehow grown uncontrollably.</t>
-  </si>
-  <si>
     <t>We must find a way to shrink them back!</t>
   </si>
   <si>
@@ -490,9 +448,6 @@
     <t>intro_op_2</t>
   </si>
   <si>
-    <t>According to the latest studies of blobology, the only way to shrink them is by the power of the divide operation.</t>
-  </si>
-  <si>
     <t>Divide and conquer, as they say!</t>
   </si>
   <si>
@@ -520,12 +475,6 @@
     <t>Let’s briefly examine a useful mathematical principle to help us.</t>
   </si>
   <si>
-    <t>Now with that in mind, we can split the dividend up by this principle.</t>
-  </si>
-  <si>
-    <t>Pay close attention to how the distributive property works!</t>
-  </si>
-  <si>
     <t>Let’s go ahead and put this into practice when we face the mega blob!</t>
   </si>
   <si>
@@ -556,21 +505,9 @@
     <t>Once all the blobs have been merged into the final quotient blob, we will be able to attack.</t>
   </si>
   <si>
-    <t>Here we are going to reduce the blob’s large number by multiplying the divisor with a number.</t>
-  </si>
-  <si>
-    <t>First you must specify the number to multiply the divisor. Simply type in the number, and press ENTER.</t>
-  </si>
-  <si>
     <t>Now you must type in the correct answer for the multiplication.</t>
   </si>
   <si>
-    <t>Splitting up large numbers this way will make it easier to deal with two or more-digit divisors!</t>
-  </si>
-  <si>
-    <t>I’ve said everything that I can to help you, the rest is up to you. Go forth, and defeat the mega blobs!</t>
-  </si>
-  <si>
     <t>In order to beat the mega blob, we must merge all the blobs into one final quotient blob.</t>
   </si>
   <si>
@@ -590,6 +527,141 @@
   </si>
   <si>
     <t>Fortunately, we have one more trick up our sleeves!</t>
+  </si>
+  <si>
+    <t>It seems these blobs came from a lab and have somehow grown uncontrollably.</t>
+  </si>
+  <si>
+    <t>According to the latest studies of blob-ology, the only way to shrink them is by the power of the division operation.</t>
+  </si>
+  <si>
+    <t>These digits are placed by multiples of 10, since we use a base 10 number system.</t>
+  </si>
+  <si>
+    <t>lesson1_placeValueDist_0</t>
+  </si>
+  <si>
+    <t>lesson1_digitSwapFirst_0</t>
+  </si>
+  <si>
+    <t>lesson1_digitSwapFirst_1</t>
+  </si>
+  <si>
+    <t>lesson1_digitSwapSecond_0</t>
+  </si>
+  <si>
+    <t>lesson1_digitSwapComplete_0</t>
+  </si>
+  <si>
+    <t>lesson1_digitSwapComplete_1</t>
+  </si>
+  <si>
+    <t>As you can see, we now have two divisions that are much easier to solve.</t>
+  </si>
+  <si>
+    <t>Press each one to solve the division.</t>
+  </si>
+  <si>
+    <t>lesson1_divisionsSolved_0</t>
+  </si>
+  <si>
+    <t>lesson1_divisionsSolved_1</t>
+  </si>
+  <si>
+    <t>Now we just have to add both numbers to get the final answer.</t>
+  </si>
+  <si>
+    <t>Why don’t you do the honors by pressing on the plus sign.</t>
+  </si>
+  <si>
+    <t>lesson1_addSolved_0</t>
+  </si>
+  <si>
+    <t>lesson1_addSolved_1</t>
+  </si>
+  <si>
+    <t>Let’s put this into practice by splitting up the large number. Drag the equation all the way to the left.</t>
+  </si>
+  <si>
+    <t>Now we can start moving the digits from one number into another.</t>
+  </si>
+  <si>
+    <t>Press the highlighted digit to make the move.</t>
+  </si>
+  <si>
+    <t>Now for the next digit, moving this will still make both numbers wholly divisible.</t>
+  </si>
+  <si>
+    <t>Not bad! As you can see, splitting up a large number this way can help solve divisions easily.</t>
+  </si>
+  <si>
+    <t>lesson2_areaModel_drag_0</t>
+  </si>
+  <si>
+    <t>lesson2_areaModel_drag_1</t>
+  </si>
+  <si>
+    <t>Drag the area from left to right to see how this works.</t>
+  </si>
+  <si>
+    <t>lesson2_areaModel_drag_complete_0</t>
+  </si>
+  <si>
+    <t>lesson2_areaModel_drag_complete_1</t>
+  </si>
+  <si>
+    <t>As you can see, each number multiplied by 12, the divisor, is subtracted from the dividend.</t>
+  </si>
+  <si>
+    <t>Now we can easily divide the remaining dividend to get the final answer.</t>
+  </si>
+  <si>
+    <t>lesson2_areaModel_answer_0</t>
+  </si>
+  <si>
+    <t>split_op_partial_mult_tens</t>
+  </si>
+  <si>
+    <t>Press the left button until the number is 100.</t>
+  </si>
+  <si>
+    <t>split_op_partial_mult_digit</t>
+  </si>
+  <si>
+    <t>Now press the up button until the number is 200.</t>
+  </si>
+  <si>
+    <t>split_op_partial_next</t>
+  </si>
+  <si>
+    <t>Press this button to proceed.</t>
+  </si>
+  <si>
+    <t>level3_intro_1</t>
+  </si>
+  <si>
+    <t>Just as you have done before, press the sparkly blob to commence the split.</t>
+  </si>
+  <si>
+    <t>The best approach is to multiply a single number by 10 several times, as long as it’s not larger than the dividend.</t>
+  </si>
+  <si>
+    <t>split_op_partial_instruct_2</t>
+  </si>
+  <si>
+    <t>We will do exactly that for this problem!</t>
+  </si>
+  <si>
+    <t>Now we are going to reduce the dividend blob’s number by multiplying the divisor blob with a number.</t>
+  </si>
+  <si>
+    <t>We’ll be employing the area model trick we just learned to defeat this blob.</t>
+  </si>
+  <si>
+    <t>Splitting up large numbers this way will make it easier to deal with two or more-digit divisors.</t>
+  </si>
+  <si>
+    <t>Remember this trick, and you will be able to defeat these mega blobs with ease!</t>
   </si>
 </sst>
 </file>
@@ -925,10 +997,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D94"/>
+  <dimension ref="A1:D106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -963,82 +1035,82 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -1107,18 +1179,18 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
       <c r="B21" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="B22" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -1171,106 +1243,106 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B29" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B30" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="B31" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="B32" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="B33" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="B34" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="B35" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="B36" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="B37" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="B38" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="B39" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="B40" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="B41" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
@@ -1286,7 +1358,7 @@
         <v>34</v>
       </c>
       <c r="B43" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
@@ -1302,407 +1374,503 @@
         <v>39</v>
       </c>
       <c r="B45" t="s">
-        <v>40</v>
+        <v>171</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>41</v>
+        <v>172</v>
       </c>
       <c r="B46" t="s">
-        <v>166</v>
+        <v>186</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>42</v>
+        <v>173</v>
       </c>
       <c r="B47" t="s">
-        <v>45</v>
+        <v>187</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>44</v>
+        <v>174</v>
       </c>
       <c r="B48" t="s">
-        <v>167</v>
+        <v>188</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>43</v>
+        <v>175</v>
       </c>
       <c r="B49" t="s">
-        <v>168</v>
+        <v>189</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>50</v>
+        <v>176</v>
       </c>
       <c r="B50" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>177</v>
       </c>
       <c r="B51" t="s">
-        <v>58</v>
+        <v>179</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>59</v>
+        <v>180</v>
       </c>
       <c r="B52" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>181</v>
       </c>
       <c r="B53" t="s">
-        <v>60</v>
+        <v>183</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>184</v>
       </c>
       <c r="B54" t="s">
-        <v>170</v>
+        <v>190</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>185</v>
       </c>
       <c r="B55" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B56" t="s">
-        <v>61</v>
+        <v>152</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="B57" t="s">
-        <v>172</v>
+        <v>49</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B58" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="B59" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="B60" t="s">
-        <v>183</v>
+        <v>153</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>65</v>
+        <v>191</v>
       </c>
       <c r="B61" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>66</v>
+        <v>192</v>
       </c>
       <c r="B62" t="s">
-        <v>67</v>
+        <v>193</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>68</v>
+        <v>194</v>
       </c>
       <c r="B63" t="s">
-        <v>71</v>
+        <v>196</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>69</v>
+        <v>195</v>
       </c>
       <c r="B64" t="s">
-        <v>72</v>
+        <v>197</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>70</v>
+        <v>198</v>
       </c>
       <c r="B65" t="s">
-        <v>73</v>
+        <v>155</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="B66" t="s">
-        <v>184</v>
+        <v>156</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="B67" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="B68" t="s">
-        <v>79</v>
+        <v>162</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="B69" t="s">
-        <v>80</v>
+        <v>157</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="B70" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="B71" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="B72" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>89</v>
+        <v>60</v>
       </c>
       <c r="B73" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="B74" t="s">
-        <v>85</v>
+        <v>163</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="B75" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="B76" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="B77" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="B78" t="s">
-        <v>175</v>
+        <v>76</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="B79" t="s">
-        <v>176</v>
+        <v>77</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
+        <v>73</v>
+      </c>
+      <c r="B80" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>79</v>
+      </c>
+      <c r="B81" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>80</v>
+      </c>
+      <c r="B82" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>81</v>
+      </c>
+      <c r="B83" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>82</v>
+      </c>
+      <c r="B84" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>83</v>
+      </c>
+      <c r="B85" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>87</v>
+      </c>
+      <c r="B86" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>88</v>
+      </c>
+      <c r="B87" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>89</v>
+      </c>
+      <c r="B88" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>90</v>
+      </c>
+      <c r="B89" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>92</v>
+      </c>
+      <c r="B90" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>205</v>
+      </c>
+      <c r="B91" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>94</v>
+      </c>
+      <c r="B92" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>95</v>
+      </c>
+      <c r="B93" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>96</v>
+      </c>
+      <c r="B94" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>208</v>
+      </c>
+      <c r="B95" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>199</v>
+      </c>
+      <c r="B96" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>201</v>
+      </c>
+      <c r="B97" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>203</v>
+      </c>
+      <c r="B98" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>97</v>
+      </c>
+      <c r="B99" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>98</v>
+      </c>
+      <c r="B100" t="s">
         <v>99</v>
       </c>
-      <c r="B80" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
         <v>100</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B101" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
+      <c r="B102" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
         <v>102</v>
       </c>
-      <c r="B82" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
-        <v>104</v>
-      </c>
-      <c r="B83" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
-        <v>106</v>
-      </c>
-      <c r="B84" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
-        <v>107</v>
-      </c>
-      <c r="B85" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
-        <v>108</v>
-      </c>
-      <c r="B86" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
-        <v>109</v>
-      </c>
-      <c r="B87" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
-        <v>110</v>
-      </c>
-      <c r="B88" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A89" t="s">
-        <v>113</v>
-      </c>
-      <c r="B89" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A90" t="s">
-        <v>114</v>
-      </c>
-      <c r="B90" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
-        <v>115</v>
-      </c>
-      <c r="B91" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
-        <v>159</v>
-      </c>
-      <c r="B92" t="s">
-        <v>160</v>
-      </c>
-      <c r="C92">
+      <c r="B103" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>144</v>
+      </c>
+      <c r="B104" t="s">
+        <v>145</v>
+      </c>
+      <c r="C104">
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
-        <v>161</v>
-      </c>
-      <c r="B93" t="s">
-        <v>162</v>
-      </c>
-      <c r="C93">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>146</v>
+      </c>
+      <c r="B105" t="s">
+        <v>147</v>
+      </c>
+      <c r="C105">
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A94" t="s">
-        <v>164</v>
-      </c>
-      <c r="B94" t="s">
-        <v>163</v>
-      </c>
-      <c r="C94">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>149</v>
+      </c>
+      <c r="B106" t="s">
+        <v>148</v>
+      </c>
+      <c r="C106">
         <v>2</v>
       </c>
     </row>

</xml_diff>